<commit_message>
Flere forbedringer til baneallokering
- Fikset sluttspillbane-markering for både 'stuttspil' og 'sluttspil'
- Slått sammen Drammenshallen stuttspillbaner A/B/C/D til én bane
- Implementert visuell indikasjon for baner uten kapasitet under drag
  - Baner uten nok plass eller med klister-konflikt gråes ut
  - Drop forhindres på baner uten kapasitet
- Fikset bug hvor alle puljer dukket opp igjen ved sletting
  - displayPools() filtrerer nå bort allerede allokerte puljer
  - Ved sletting legges kun den slettede puljen tilbake

Forbedrer brukeropplevelsen ved å gi tydeligere tilbakemeldinger og forhindre feil.

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/hallkapasitet.xlsx
+++ b/hallkapasitet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomashm/projects/personal/dhc2025-hall-puljer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861D9D57-602C-104A-815E-1AABD4EE3424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B428725-A71E-934F-996F-32D73BA4D8C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5260" yWindow="4660" windowWidth="26040" windowHeight="14940" xr2:uid="{551327EB-5E80-7B48-84F1-55FB71A1F25D}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="53">
   <si>
     <t>Anlegg</t>
   </si>
@@ -173,6 +173,9 @@
     <t>Kommentar</t>
   </si>
   <si>
+    <t>fre 18–22;lør 08–21</t>
+  </si>
+  <si>
     <t>fre 18–22;lør 08–21;søn 08–17</t>
   </si>
   <si>
@@ -186,6 +189,15 @@
   </si>
   <si>
     <t>søn 13–17</t>
+  </si>
+  <si>
+    <t>Brandenga-Sluttspillbane 1</t>
+  </si>
+  <si>
+    <t>Sluttspillbane 1</t>
+  </si>
+  <si>
+    <t>Konnerud-Sluttspillbane 1</t>
   </si>
 </sst>
 </file>
@@ -558,9 +570,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63AD7C43-2826-2545-ADA3-B74EC7F9C3B2}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -612,7 +626,7 @@
         <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H2">
         <v>1560</v>
@@ -632,7 +646,7 @@
         <v>40</v>
       </c>
       <c r="G3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H3">
         <v>1560</v>
@@ -640,66 +654,65 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H4">
-        <v>1560</v>
+        <v>540</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H5">
-        <v>840</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="1"/>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H6">
         <v>840</v>
@@ -707,13 +720,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>39</v>
@@ -723,7 +736,7 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H7">
         <v>840</v>
@@ -731,19 +744,23 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
         <v>39</v>
       </c>
+      <c r="E8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="1"/>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H8">
         <v>840</v>
@@ -751,36 +768,33 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G9" t="s">
         <v>46</v>
       </c>
       <c r="H9">
-        <v>540</v>
+        <v>840</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
         <v>38</v>
@@ -792,18 +806,18 @@
         <v>47</v>
       </c>
       <c r="H10">
-        <v>285</v>
+        <v>540</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
         <v>38</v>
@@ -815,18 +829,18 @@
         <v>48</v>
       </c>
       <c r="H11">
-        <v>240</v>
+        <v>285</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
         <v>38</v>
@@ -835,21 +849,21 @@
         <v>41</v>
       </c>
       <c r="G12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H12">
-        <v>285</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
         <v>38</v>
@@ -858,59 +872,105 @@
         <v>41</v>
       </c>
       <c r="G13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H13">
-        <v>540</v>
+        <v>285</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
       </c>
       <c r="G14" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H14">
-        <v>1560</v>
+        <v>540</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>23</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>4</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C17" t="s">
         <v>3</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D17" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G15" t="s">
-        <v>44</v>
-      </c>
-      <c r="H15">
+      <c r="G17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17">
         <v>1560</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G15" xr:uid="{63AD7C43-2826-2545-ADA3-B74EC7F9C3B2}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G15">
-      <sortCondition ref="A1:A15"/>
+  <autoFilter ref="A1:G17" xr:uid="{63AD7C43-2826-2545-ADA3-B74EC7F9C3B2}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G17">
+      <sortCondition ref="A1:A17"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>